<commit_message>
Updated For Python 3.9.7
- Changed Relative to Absolute Imports
- Updated Deprecated Function "np.asscalar"
</commit_message>
<xml_diff>
--- a/IBT Liability & SC Returns & PV.xlsx
+++ b/IBT Liability & SC Returns & PV.xlsx
@@ -397,7 +397,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.009428657168074173</v>
+        <v>0.00941189106787399</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -405,7 +405,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-0.007215625535114567</v>
+        <v>-0.007233637626833378</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -413,7 +413,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-0.008876482286584109</v>
+        <v>-0.008886374037158085</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -421,7 +421,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.03677437797087402</v>
+        <v>0.03682809900623907</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -429,7 +429,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>-0.004952192512322928</v>
+        <v>-0.004959321813804207</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -437,7 +437,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.0512721059994643</v>
+        <v>0.05134596372618505</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -445,7 +445,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.01063887559584842</v>
+        <v>0.01063085219126325</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -453,7 +453,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.0575074062083889</v>
+        <v>0.05757928115043698</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -461,7 +461,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-0.01388598071628111</v>
+        <v>-0.01391105474125276</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -469,7 +469,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-0.03791581397484978</v>
+        <v>-0.03799018815254573</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -477,7 +477,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-0.006560621212924667</v>
+        <v>-0.006551045640652231</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -485,7 +485,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-0.01638838572634371</v>
+        <v>-0.01637038860987938</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -493,7 +493,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-0.03110373411559697</v>
+        <v>-0.03116921229449932</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -501,7 +501,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.01693362146853561</v>
+        <v>0.01696658957243891</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -509,7 +509,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>-0.0138167844213114</v>
+        <v>-0.0138355666305976</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -517,7 +517,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.02300584044092346</v>
+        <v>0.02302740684578586</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -525,7 +525,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.0185198215086213</v>
+        <v>0.01853808067085527</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -533,7 +533,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>-0.02788495512599876</v>
+        <v>-0.02792268862873748</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -541,7 +541,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.04631350110954591</v>
+        <v>0.04636814787205168</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -549,7 +549,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.02318590421389999</v>
+        <v>0.02321602492463759</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -557,7 +557,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.07338928849327986</v>
+        <v>0.07356439076592203</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -565,7 +565,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>-0.0004452045179317299</v>
+        <v>-0.0004548069691432399</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -573,7 +573,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.00060605403993641</v>
+        <v>0.0006175479654066951</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -581,7 +581,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.04557451014239078</v>
+        <v>0.04563447144403843</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -589,7 +589,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>-0.004074166107454258</v>
+        <v>-0.00411997300826028</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -597,7 +597,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.001946508633915212</v>
+        <v>0.001951633937907093</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -605,7 +605,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>-0.03515937190575658</v>
+        <v>-0.03520674959291892</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -613,7 +613,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0.02134595782907689</v>
+        <v>0.02135597270618761</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -621,7 +621,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0.0316994260116823</v>
+        <v>0.03175009444753618</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -629,7 +629,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.03453241642638982</v>
+        <v>0.03459765643091917</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -637,7 +637,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.06688927574848202</v>
+        <v>0.06700006463050312</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -645,7 +645,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>-0.01486782569019607</v>
+        <v>-0.01490621294669192</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -653,7 +653,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>-0.01708452310267672</v>
+        <v>-0.0171134510957166</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -661,7 +661,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0.01868940751270154</v>
+        <v>0.01871199575682403</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -669,7 +669,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>-0.01278082313719697</v>
+        <v>-0.01280384060965067</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -677,7 +677,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>-0.02240267188180156</v>
+        <v>-0.02244115589196882</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -685,7 +685,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>-0.04006841670029448</v>
+        <v>-0.04011259000418044</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -693,7 +693,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>0.007695368336138264</v>
+        <v>0.007699959297102099</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -701,7 +701,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>-0.009302478128019875</v>
+        <v>-0.009320920318550585</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -709,7 +709,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0.04084194025033971</v>
+        <v>0.04090664447161108</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -717,7 +717,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>-0.06731292630033325</v>
+        <v>-0.06739838990174729</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -725,7 +725,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>-0.04769985500717389</v>
+        <v>-0.04775481204572551</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -733,7 +733,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>-0.001491390881913857</v>
+        <v>-0.001491783788181933</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -741,7 +741,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>-0.007420572905411982</v>
+        <v>-0.007417966471515824</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -749,7 +749,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>-0.007000848442292873</v>
+        <v>-0.00703521844348709</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -757,7 +757,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>0.01703913730286954</v>
+        <v>0.01705539420938829</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -765,7 +765,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>-0.01727895126830659</v>
+        <v>-0.01730097187329915</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -773,7 +773,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>-0.005302340150941665</v>
+        <v>-0.005295026615631526</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -781,7 +781,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>0.04179692196453821</v>
+        <v>0.04186191849029752</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -789,7 +789,7 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>0.01432744673505559</v>
+        <v>0.01434962396996919</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -797,7 +797,7 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>0.005673735782825595</v>
+        <v>0.005694246995680663</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -805,7 +805,7 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>0.01671030518831773</v>
+        <v>0.01673526805109704</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -813,7 +813,7 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>0.01901753857626898</v>
+        <v>0.01903370881767263</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -821,7 +821,7 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>-0.002953169644868581</v>
+        <v>-0.002950600694963224</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -829,7 +829,7 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>4.071697806895536E-05</v>
+        <v>4.742876610164259E-05</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -837,7 +837,7 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>0.03574681356191189</v>
+        <v>0.03579929811518623</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -845,7 +845,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>-0.03334449366931858</v>
+        <v>-0.0333870741929706</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -853,7 +853,7 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>0.02047395025467802</v>
+        <v>0.02050585873458965</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -861,7 +861,7 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>0.0177594674466397</v>
+        <v>0.01778369672416868</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -869,7 +869,7 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>0.02038370464172878</v>
+        <v>0.02043034787221254</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -877,7 +877,7 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>0.08127655689697111</v>
+        <v>0.08141252914529074</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -885,7 +885,7 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>-0.04541177714667599</v>
+        <v>-0.0454889276391186</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -893,7 +893,7 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>0.001704094322653615</v>
+        <v>0.001709458790571716</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -901,7 +901,7 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>-0.03167676196247016</v>
+        <v>-0.03173642251707964</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -909,7 +909,7 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>-0.02994987795985415</v>
+        <v>-0.03000140517583527</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -917,7 +917,7 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>-0.045314230682312</v>
+        <v>-0.04537654585800455</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -925,7 +925,7 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>0.02112032055577839</v>
+        <v>0.02115561179613445</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -933,7 +933,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>-0.01239252695960569</v>
+        <v>-0.0124067842460569</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -941,7 +941,7 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>0.01028795977911612</v>
+        <v>0.01028814243065224</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -949,7 +949,7 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>0.002529809279722794</v>
+        <v>0.002533062514028517</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -957,7 +957,7 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>-0.001816438906292128</v>
+        <v>-0.001817354607100974</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -965,7 +965,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>-0.004424072438801052</v>
+        <v>-0.004424108122885184</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -973,7 +973,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>0.008913549135156629</v>
+        <v>0.008915729771647118</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -981,7 +981,7 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>0.02303541876307236</v>
+        <v>0.02307161281381997</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -989,7 +989,7 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>0.03810769859349894</v>
+        <v>0.03815639563387219</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -997,7 +997,7 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>0.0154053833534844</v>
+        <v>0.01543004597713904</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1005,7 +1005,7 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>-0.00544279196197639</v>
+        <v>-0.005447066411527701</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1013,7 +1013,7 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>0.04386318520714427</v>
+        <v>0.04391646600747068</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1021,7 +1021,7 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>0.02466087568558573</v>
+        <v>0.02469951584133701</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1029,7 +1029,7 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>-0.0005822137264527294</v>
+        <v>-0.0005704850537233686</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1037,7 +1037,7 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>-0.01881460787750944</v>
+        <v>-0.01884427784079812</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1045,7 +1045,7 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>-0.03379804845614776</v>
+        <v>-0.03384684445225183</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1053,7 +1053,7 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>-0.06106677142295136</v>
+        <v>-0.06113559257627732</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1061,7 +1061,7 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>-0.0004281493204609799</v>
+        <v>-0.0004153665778678928</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1069,7 +1069,7 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>-0.003230441345088986</v>
+        <v>-0.003235115675846667</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1077,7 +1077,7 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>0.02026408046596417</v>
+        <v>0.02029176073849026</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1085,7 +1085,7 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>-0.01324499518268074</v>
+        <v>-0.01326316982782771</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1093,7 +1093,7 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>0.01429784962941949</v>
+        <v>0.01431105676113642</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1101,7 +1101,7 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>0.01967021305615857</v>
+        <v>0.01970073973434894</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1109,7 +1109,7 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>0.006313398526782255</v>
+        <v>0.006336096846517147</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1117,7 +1117,7 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>0.003537826788374998</v>
+        <v>0.003537772688336771</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1125,7 +1125,7 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>0.01534019698703593</v>
+        <v>0.01535941852970679</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1133,7 +1133,7 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>-0.01118134664421822</v>
+        <v>-0.01118837781197912</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1141,7 +1141,7 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>0.006919972069649338</v>
+        <v>0.006934937124762897</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1149,7 +1149,7 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>-0.0002357038271636469</v>
+        <v>-0.0002234492626821405</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1157,7 +1157,7 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>0.0287241695157916</v>
+        <v>0.02877763874906702</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1165,7 +1165,7 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>-0.03125711777301443</v>
+        <v>-0.03128748513955992</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1173,7 +1173,7 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>-0.03707685472017186</v>
+        <v>-0.03712585797545243</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1181,7 +1181,7 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>0.007787192515962271</v>
+        <v>0.007803716606547439</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1189,7 +1189,7 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>-0.0199848716537363</v>
+        <v>-0.02000922776167302</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1197,7 +1197,7 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>0.009528148518190838</v>
+        <v>0.00953953285139697</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1205,7 +1205,7 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>-0.01919454211402638</v>
+        <v>-0.01921615188353332</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1213,7 +1213,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>0.006346257825524892</v>
+        <v>0.00635902180738479</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1221,7 +1221,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>0.00590847876236622</v>
+        <v>0.005910900146230524</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1229,7 +1229,7 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>-0.01812741088363312</v>
+        <v>-0.01814701228498561</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1237,7 +1237,7 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>-0.04182593136233581</v>
+        <v>-0.04189219979904812</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1245,7 +1245,7 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>0.0004261562397547269</v>
+        <v>0.0004252532631316974</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1253,7 +1253,7 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>0.0372655978271681</v>
+        <v>0.03731835606704648</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1261,7 +1261,7 @@
         <v>108</v>
       </c>
       <c r="B110">
-        <v>0.02642575772024802</v>
+        <v>0.02644732996213528</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1269,7 +1269,7 @@
         <v>109</v>
       </c>
       <c r="B111">
-        <v>-0.0078271711054273</v>
+        <v>-0.007838426081494876</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1277,7 +1277,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>0.04831183531742589</v>
+        <v>0.04837236707905013</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1285,7 +1285,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>-0.01340654551019915</v>
+        <v>-0.01342672550647295</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1293,7 +1293,7 @@
         <v>112</v>
       </c>
       <c r="B114">
-        <v>0.03861851805966321</v>
+        <v>0.0386705639416427</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1301,7 +1301,7 @@
         <v>113</v>
       </c>
       <c r="B115">
-        <v>0.0319355786543134</v>
+        <v>0.03197295042769421</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1309,7 +1309,7 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>0.0122879832327214</v>
+        <v>0.01230767104346664</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1317,7 +1317,7 @@
         <v>115</v>
       </c>
       <c r="B117">
-        <v>0.08081294626213942</v>
+        <v>0.08093752404074883</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1325,7 +1325,7 @@
         <v>116</v>
       </c>
       <c r="B118">
-        <v>-0.02424463653545161</v>
+        <v>-0.02427711429090307</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1333,7 +1333,7 @@
         <v>117</v>
       </c>
       <c r="B119">
-        <v>0.0001345761816897717</v>
+        <v>0.0001286320091367088</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1341,7 +1341,7 @@
         <v>118</v>
       </c>
       <c r="B120">
-        <v>-0.0002756117553136539</v>
+        <v>-0.000265446909045286</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1349,7 +1349,7 @@
         <v>119</v>
       </c>
       <c r="B121">
-        <v>-0.01603670893605613</v>
+        <v>-0.01606324099728251</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -1357,7 +1357,7 @@
         <v>120</v>
       </c>
       <c r="B122">
-        <v>0.05794455724586034</v>
+        <v>0.05802516151895576</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -1365,7 +1365,7 @@
         <v>121</v>
       </c>
       <c r="B123">
-        <v>0.0294377560270811</v>
+        <v>0.0294739757326552</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1373,7 +1373,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>-0.0662817548006216</v>
+        <v>-0.06634599121424234</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1381,7 +1381,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>0.0646974307870043</v>
+        <v>0.06474709905174048</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1389,7 +1389,7 @@
         <v>124</v>
       </c>
       <c r="B126">
-        <v>0.006057074559889575</v>
+        <v>0.006035001200904277</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1397,7 +1397,7 @@
         <v>125</v>
       </c>
       <c r="B127">
-        <v>0.01456205400967114</v>
+        <v>0.01458434541256004</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1405,7 +1405,7 @@
         <v>126</v>
       </c>
       <c r="B128">
-        <v>0.07633640542490405</v>
+        <v>0.07645807577643038</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1413,7 +1413,7 @@
         <v>127</v>
       </c>
       <c r="B129">
-        <v>-0.06243790900984991</v>
+        <v>-0.06254227675749868</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -1421,7 +1421,7 @@
         <v>128</v>
       </c>
       <c r="B130">
-        <v>0.001130384896524506</v>
+        <v>0.001137207550270691</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1429,7 +1429,7 @@
         <v>129</v>
       </c>
       <c r="B131">
-        <v>-0.02376523484538395</v>
+        <v>-0.02380283607536993</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -1437,7 +1437,7 @@
         <v>130</v>
       </c>
       <c r="B132">
-        <v>0.05175178969128091</v>
+        <v>0.05184752223383349</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1445,7 +1445,7 @@
         <v>131</v>
       </c>
       <c r="B133">
-        <v>-0.003980024895629319</v>
+        <v>-0.003985862784610439</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -1453,7 +1453,7 @@
         <v>132</v>
       </c>
       <c r="B134">
-        <v>-0.03914707835635312</v>
+        <v>-0.03920646205956757</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -1461,7 +1461,7 @@
         <v>133</v>
       </c>
       <c r="B135">
-        <v>-0.0466843624164307</v>
+        <v>-0.04674215976482576</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -1469,7 +1469,7 @@
         <v>134</v>
       </c>
       <c r="B136">
-        <v>-0.04025468867354909</v>
+        <v>-0.04029902656457207</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -1477,7 +1477,7 @@
         <v>135</v>
       </c>
       <c r="B137">
-        <v>0.02425033353671369</v>
+        <v>0.02428305824716515</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -1485,7 +1485,7 @@
         <v>136</v>
       </c>
       <c r="B138">
-        <v>0.002709149299492397</v>
+        <v>0.002708048971293175</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -1493,7 +1493,7 @@
         <v>137</v>
       </c>
       <c r="B139">
-        <v>0.04292388907637323</v>
+        <v>0.04300061205157379</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -1501,7 +1501,7 @@
         <v>138</v>
       </c>
       <c r="B140">
-        <v>0.02484444652838547</v>
+        <v>0.02487547825832648</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -1509,7 +1509,7 @@
         <v>139</v>
       </c>
       <c r="B141">
-        <v>-0.00913812607372344</v>
+        <v>-0.009147539353638545</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -1517,7 +1517,7 @@
         <v>140</v>
       </c>
       <c r="B142">
-        <v>-0.02259384490101424</v>
+        <v>-0.02262158528885805</v>
       </c>
     </row>
   </sheetData>
@@ -1543,7 +1543,7 @@
         <v>40178</v>
       </c>
       <c r="B2">
-        <v>9441977545.491364</v>
+        <v>9467109549.975756</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1551,7 +1551,7 @@
         <v>40209</v>
       </c>
       <c r="B3">
-        <v>9531002714.756456</v>
+        <v>9556212953.787758</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1559,7 +1559,7 @@
         <v>40237</v>
       </c>
       <c r="B4">
-        <v>9462230568.192614</v>
+        <v>9487086772.195206</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1567,7 +1567,7 @@
         <v>40268</v>
       </c>
       <c r="B5">
-        <v>9378239246.162477</v>
+        <v>9402780970.614504</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1575,7 +1575,7 @@
         <v>40298</v>
       </c>
       <c r="B6">
-        <v>9723118160.902142</v>
+        <v>9749067519.134275</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1583,7 +1583,7 @@
         <v>40329</v>
       </c>
       <c r="B7">
-        <v>9674967407.949291</v>
+        <v>9700718755.922382</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1591,7 +1591,7 @@
         <v>40359</v>
       </c>
       <c r="B8">
-        <v>10171023362.43103</v>
+        <v>10198811509.2819</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1599,7 +1599,7 @@
         <v>40390</v>
       </c>
       <c r="B9">
-        <v>10279231614.6664</v>
+        <v>10307233566.96363</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1607,7 +1607,7 @@
         <v>40421</v>
       </c>
       <c r="B10">
-        <v>10870363562.64113</v>
+        <v>10900716666.39905</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1615,7 +1615,7 @@
         <v>40451</v>
       </c>
       <c r="B11">
-        <v>10719417903.83134</v>
+        <v>10749076200.13388</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1623,7 +1623,7 @@
         <v>40482</v>
       </c>
       <c r="B12">
-        <v>10312982448.67099</v>
+        <v>10340716772.82475</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1631,7 +1631,7 @@
         <v>40512</v>
       </c>
       <c r="B13">
-        <v>10245322877.24972</v>
+        <v>10272974265.28891</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1639,7 +1639,7 @@
         <v>40543</v>
       </c>
       <c r="B14">
-        <v>10077418574.04642</v>
+        <v>10104801684.38684</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1647,7 +1647,7 @@
         <v>40574</v>
       </c>
       <c r="B15">
-        <v>9763973226.147701</v>
+        <v>9789842975.492376</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1655,7 +1655,7 @@
         <v>40602</v>
       </c>
       <c r="B16">
-        <v>9929312652.788202</v>
+        <v>9955943223.236179</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1663,7 +1663,7 @@
         <v>40633</v>
       </c>
       <c r="B17">
-        <v>9792121480.412828</v>
+        <v>9818197107.400648</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1671,7 +1671,7 @@
         <v>40663</v>
       </c>
       <c r="B18">
-        <v>10017397464.76935</v>
+        <v>10044284726.68488</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1679,7 +1679,7 @@
         <v>40694</v>
       </c>
       <c r="B19">
-        <v>10202917877.79779</v>
+        <v>10230486487.22921</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1687,7 +1687,7 @@
         <v>40724</v>
       </c>
       <c r="B20">
-        <v>9918409970.621149</v>
+        <v>9944823798.525799</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1695,7 +1695,7 @@
         <v>40755</v>
       </c>
       <c r="B21">
-        <v>10377766261.80044</v>
+        <v>10405946858.97734</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1703,7 +1703,7 @@
         <v>40786</v>
       </c>
       <c r="B22">
-        <v>10618384156.30079</v>
+        <v>10647531580.61981</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1711,7 +1711,7 @@
         <v>40816</v>
       </c>
       <c r="B23">
-        <v>11397659814.48002</v>
+        <v>11430810754.50903</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1719,7 +1719,7 @@
         <v>40847</v>
       </c>
       <c r="B24">
-        <v>11392585524.83677</v>
+        <v>11425611942.11492</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1727,7 +1727,7 @@
         <v>40877</v>
       </c>
       <c r="B25">
-        <v>11399490047.31942</v>
+        <v>11432667805.5233</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1735,7 +1735,7 @@
         <v>40908</v>
       </c>
       <c r="B26">
-        <v>11919016222.09906</v>
+        <v>11954391558.02363</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1743,7 +1743,7 @@
         <v>40939</v>
       </c>
       <c r="B27">
-        <v>11870456170.17279</v>
+        <v>11905139787.47439</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1751,7 +1751,7 @@
         <v>40968</v>
       </c>
       <c r="B28">
-        <v>11893562115.59654</v>
+        <v>11928374262.31916</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1759,7 +1759,7 @@
         <v>40999</v>
       </c>
       <c r="B29">
-        <v>11475391941.89006</v>
+        <v>11508414976.61507</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1767,7 +1767,7 @@
         <v>41029</v>
       </c>
       <c r="B30">
-        <v>11720345174.35378</v>
+        <v>11754188372.74714</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1775,7 +1775,7 @@
         <v>41060</v>
       </c>
       <c r="B31">
-        <v>12091873389.03959</v>
+        <v>12127384963.73599</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1783,7 +1783,7 @@
         <v>41090</v>
       </c>
       <c r="B32">
-        <v>12509434996.28508</v>
+        <v>12546964062.11683</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1791,7 +1791,7 @@
         <v>41121</v>
       </c>
       <c r="B33">
-        <v>13346182043.20931</v>
+        <v>13387611465.19525</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1799,7 +1799,7 @@
         <v>41152</v>
       </c>
       <c r="B34">
-        <v>13147753334.96125</v>
+        <v>13188052877.84748</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1807,7 +1807,7 @@
         <v>41182</v>
       </c>
       <c r="B35">
-        <v>12923130239.36181</v>
+        <v>12962359779.87471</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1815,7 +1815,7 @@
         <v>41213</v>
       </c>
       <c r="B36">
-        <v>13164655886.74496</v>
+        <v>13204911401.07415</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1823,7 +1823,7 @@
         <v>41243</v>
       </c>
       <c r="B37">
-        <v>12996400748.19441</v>
+        <v>13035837820.23024</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1831,7 +1831,7 @@
         <v>41274</v>
       </c>
       <c r="B38">
-        <v>12705246646.58821</v>
+        <v>12743298551.52403</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1839,7 +1839,7 @@
         <v>41305</v>
       </c>
       <c r="B39">
-        <v>12196167529.6727</v>
+        <v>12232131841.42588</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1847,7 +1847,7 @@
         <v>41333</v>
       </c>
       <c r="B40">
-        <v>12290021531.10278</v>
+        <v>12326318758.72165</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1855,7 +1855,7 @@
         <v>41364</v>
       </c>
       <c r="B41">
-        <v>12175693874.6168</v>
+        <v>12211426123.75055</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1863,7 +1863,7 @@
         <v>41394</v>
       </c>
       <c r="B42">
-        <v>12672972836.35032</v>
+        <v>12710954590.68615</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1871,7 +1871,7 @@
         <v>41425</v>
       </c>
       <c r="B43">
-        <v>11819917949.81095</v>
+        <v>11854256717.15968</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1879,7 +1879,7 @@
         <v>41455</v>
       </c>
       <c r="B44">
-        <v>11256109577.40828</v>
+        <v>11288158915.68994</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1887,7 +1887,7 @@
         <v>41486</v>
       </c>
       <c r="B45">
-        <v>11239322318.21871</v>
+        <v>11271319423.2211</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1895,7 +1895,7 @@
         <v>41517</v>
       </c>
       <c r="B46">
-        <v>11155920107.54894</v>
+        <v>11187709153.6499</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1903,7 +1903,7 @@
         <v>41547</v>
       </c>
       <c r="B47">
-        <v>11077819201.64166</v>
+        <v>11109001175.87177</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1911,7 +1911,7 @@
         <v>41578</v>
       </c>
       <c r="B48">
-        <v>11266575684.0348</v>
+        <v>11298469570.19882</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1919,7 +1919,7 @@
         <v>41608</v>
       </c>
       <c r="B49">
-        <v>11071901071.82967</v>
+        <v>11102995065.95348</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1927,7 +1927,7 @@
         <v>41639</v>
       </c>
       <c r="B50">
-        <v>11013194086.22926</v>
+        <v>11044204411.56603</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1935,7 +1935,7 @@
         <v>41670</v>
       </c>
       <c r="B51">
-        <v>11473511700.0317</v>
+        <v>11506535996.4332</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1943,7 +1943,7 @@
         <v>41698</v>
       </c>
       <c r="B52">
-        <v>11637897827.77794</v>
+        <v>11671650461.17893</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1951,7 +1951,7 @@
         <v>41729</v>
       </c>
       <c r="B53">
-        <v>11703928185.12027</v>
+        <v>11738111721.75213</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1959,7 +1959,7 @@
         <v>41759</v>
       </c>
       <c r="B54">
-        <v>11899504396.99578</v>
+        <v>11934552167.82937</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1967,7 +1967,7 @@
         <v>41790</v>
       </c>
       <c r="B55">
-        <v>12125803680.90413</v>
+        <v>12161710958.66116</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1975,7 +1975,7 @@
         <v>41820</v>
       </c>
       <c r="B56">
-        <v>12089994125.55405</v>
+        <v>12125826605.85459</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1983,7 +1983,7 @@
         <v>41851</v>
       </c>
       <c r="B57">
-        <v>12090486393.57971</v>
+        <v>12126401718.84847</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1991,7 +1991,7 @@
         <v>41882</v>
       </c>
       <c r="B58">
-        <v>12522682756.56384</v>
+        <v>12560518389.04603</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1999,7 +1999,7 @@
         <v>41912</v>
       </c>
       <c r="B59">
-        <v>12105120240.66471</v>
+        <v>12141159429.68878</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -2007,7 +2007,7 @@
         <v>41943</v>
       </c>
       <c r="B60">
-        <v>12352959870.29898</v>
+        <v>12390124329.82811</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -2015,7 +2015,7 @@
         <v>41973</v>
       </c>
       <c r="B61">
-        <v>12572341858.9852</v>
+        <v>12610466543.28452</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -2023,7 +2023,7 @@
         <v>42004</v>
       </c>
       <c r="B62">
-        <v>12828612762.0936</v>
+        <v>12868102761.59472</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -2031,7 +2031,7 @@
         <v>42035</v>
       </c>
       <c r="B63">
-        <v>13871278237.16111</v>
+        <v>13915727552.71764</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -2039,7 +2039,7 @@
         <v>42063</v>
       </c>
       <c r="B64">
-        <v>13241358841.11561</v>
+        <v>13282716029.02638</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -2047,7 +2047,7 @@
         <v>42094</v>
       </c>
       <c r="B65">
-        <v>13263923365.54098</v>
+        <v>13305422284.70487</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -2055,7 +2055,7 @@
         <v>42124</v>
       </c>
       <c r="B66">
-        <v>12843765222.40229</v>
+        <v>12883155781.30931</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -2063,7 +2063,7 @@
         <v>42155</v>
       </c>
       <c r="B67">
-        <v>12459096021.44632</v>
+        <v>12496643004.77084</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -2071,7 +2071,7 @@
         <v>42185</v>
       </c>
       <c r="B68">
-        <v>11894521670.23743</v>
+        <v>11929588510.39374</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -2079,7 +2079,7 @@
         <v>42216</v>
       </c>
       <c r="B69">
-        <v>12145737780.77049</v>
+        <v>12181966253.80726</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -2087,7 +2087,7 @@
         <v>42247</v>
       </c>
       <c r="B70">
-        <v>11995221397.87799</v>
+        <v>12030827226.80353</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -2095,7 +2095,7 @@
         <v>42277</v>
       </c>
       <c r="B71">
-        <v>12118627753.16096</v>
+        <v>12154602090.87145</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -2103,7 +2103,7 @@
         <v>42308</v>
       </c>
       <c r="B72">
-        <v>12149285570.10841</v>
+        <v>12185390457.80077</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -2111,7 +2111,7 @@
         <v>42338</v>
       </c>
       <c r="B73">
-        <v>12127217135.11521</v>
+        <v>12163245282.31296</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -2119,7 +2119,7 @@
         <v>42369</v>
       </c>
       <c r="B74">
-        <v>12073565448.02839</v>
+        <v>12109433770.05884</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -2127,7 +2127,7 @@
         <v>42400</v>
       </c>
       <c r="B75">
-        <v>12181183766.88592</v>
+        <v>12217398209.24034</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -2135,7 +2135,7 @@
         <v>42429</v>
       </c>
       <c r="B76">
-        <v>12461782435.98608</v>
+        <v>12499273290.31619</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -2143,7 +2143,7 @@
         <v>42460</v>
       </c>
       <c r="B77">
-        <v>12936672284.99439</v>
+        <v>12976200507.11738</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -2151,7 +2151,7 @@
         <v>42490</v>
       </c>
       <c r="B78">
-        <v>13135966680.86313</v>
+        <v>13176423877.55078</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -2159,7 +2159,7 @@
         <v>42521</v>
       </c>
       <c r="B79">
-        <v>13064470346.99974</v>
+        <v>13104651021.62332</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -2167,7 +2167,7 @@
         <v>42551</v>
       </c>
       <c r="B80">
-        <v>13637519629.46343</v>
+        <v>13680160982.75421</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -2175,7 +2175,7 @@
         <v>42582</v>
       </c>
       <c r="B81">
-        <v>13973832805.70536</v>
+        <v>14018054335.65978</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -2183,7 +2183,7 @@
         <v>42613</v>
       </c>
       <c r="B82">
-        <v>13965697048.43473</v>
+        <v>14010057245.17901</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -2191,7 +2191,7 @@
         <v>42643</v>
       </c>
       <c r="B83">
-        <v>13702937934.73234</v>
+        <v>13746047833.88537</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -2199,7 +2199,7 @@
         <v>42674</v>
       </c>
       <c r="B84">
-        <v>13239805374.42267</v>
+        <v>13280787491.01864</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -2207,7 +2207,7 @@
         <v>42704</v>
       </c>
       <c r="B85">
-        <v>12431293205.93843</v>
+        <v>12468858677.8756</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -2215,7 +2215,7 @@
         <v>42735</v>
       </c>
       <c r="B86">
-        <v>12425970756.19986</v>
+        <v>12463679530.71665</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -2223,7 +2223,7 @@
         <v>42766</v>
       </c>
       <c r="B87">
-        <v>12385829386.51617</v>
+        <v>12423358085.6881</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -2231,7 +2231,7 @@
         <v>42794</v>
       </c>
       <c r="B88">
-        <v>12636816829.84223</v>
+        <v>12675449895.53147</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -2239,7 +2239,7 @@
         <v>42825</v>
       </c>
       <c r="B89">
-        <v>12469442251.80655</v>
+        <v>12507333250.92292</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -2247,7 +2247,7 @@
         <v>42855</v>
       </c>
       <c r="B90">
-        <v>12647728462.08562</v>
+        <v>12686326407.00732</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -2255,7 +2255,7 @@
         <v>42886</v>
       </c>
       <c r="B91">
-        <v>12896511975.61128</v>
+        <v>12936256421.73677</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -2263,7 +2263,7 @@
         <v>42916</v>
       </c>
       <c r="B92">
-        <v>12977932795.31873</v>
+        <v>13018221795.25628</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -2271,7 +2271,7 @@
         <v>42947</v>
       </c>
       <c r="B93">
-        <v>13023846473.61974</v>
+        <v>13064277304.77424</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -2279,7 +2279,7 @@
         <v>42978</v>
       </c>
       <c r="B94">
-        <v>13223634844.05398</v>
+        <v>13264937007.68642</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -2287,7 +2287,7 @@
         <v>43008</v>
       </c>
       <c r="B95">
-        <v>13075776798.96605</v>
+        <v>13116523880.79232</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -2295,7 +2295,7 @@
         <v>43039</v>
       </c>
       <c r="B96">
-        <v>13166260809.20387</v>
+        <v>13207486149.20107</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -2303,7 +2303,7 @@
         <v>43069</v>
       </c>
       <c r="B97">
-        <v>13163157471.1417</v>
+        <v>13204534946.15914</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -2311,7 +2311,7 @@
         <v>43100</v>
       </c>
       <c r="B98">
-        <v>13541258237.70584</v>
+        <v>13584530282.68914</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -2319,7 +2319,7 @@
         <v>43131</v>
       </c>
       <c r="B99">
-        <v>13117997534.17506</v>
+        <v>13159504493.3416</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -2327,7 +2327,7 @@
         <v>43159</v>
       </c>
       <c r="B100">
-        <v>12631623445.38088</v>
+        <v>12670946598.49448</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -2335,7 +2335,7 @@
         <v>43190</v>
       </c>
       <c r="B101">
-        <v>12729988328.9392</v>
+        <v>12769827074.88582</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -2343,7 +2343,7 @@
         <v>43220</v>
       </c>
       <c r="B102">
-        <v>12475581146.03179</v>
+        <v>12514312696.46725</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -2351,7 +2351,7 @@
         <v>43251</v>
       </c>
       <c r="B103">
-        <v>12594450336.04193</v>
+        <v>12633693393.54786</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -2359,7 +2359,7 @@
         <v>43281</v>
       </c>
       <c r="B104">
-        <v>12352705628.66376</v>
+        <v>12390922422.44745</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -2367,7 +2367,7 @@
         <v>43312</v>
       </c>
       <c r="B105">
-        <v>12431099083.42607</v>
+        <v>12469716568.34541</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -2375,7 +2375,7 @@
         <v>43343</v>
       </c>
       <c r="B106">
-        <v>12504547968.35336</v>
+        <v>12543423817.83269</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -2383,7 +2383,7 @@
         <v>43373</v>
       </c>
       <c r="B107">
-        <v>12277872889.41692</v>
+        <v>12315798151.7147</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -2391,7 +2391,7 @@
         <v>43404</v>
       </c>
       <c r="B108">
-        <v>11764339420.66868</v>
+        <v>11799862274.85832</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -2399,7 +2399,7 @@
         <v>43434</v>
       </c>
       <c r="B109">
-        <v>11769352867.31939</v>
+        <v>11804880204.79521</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -2407,7 +2407,7 @@
         <v>43465</v>
       </c>
       <c r="B110">
-        <v>12207944837.95895</v>
+        <v>12245418927.60659</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -2415,7 +2415,7 @@
         <v>43496</v>
       </c>
       <c r="B111">
-        <v>12530549030.509</v>
+        <v>12569277562.50957</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -2423,7 +2423,7 @@
         <v>43524</v>
       </c>
       <c r="B112">
-        <v>12432470279.20226</v>
+        <v>12470754209.43805</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -2431,7 +2431,7 @@
         <v>43555</v>
       </c>
       <c r="B113">
-        <v>13033105735.91987</v>
+        <v>13073994109.8096</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -2439,7 +2439,7 @@
         <v>43585</v>
       </c>
       <c r="B114">
-        <v>12858376810.73203</v>
+        <v>12898453179.62394</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -2447,7 +2447,7 @@
         <v>43616</v>
       </c>
       <c r="B115">
-        <v>13354948267.81524</v>
+        <v>13397243638.05487</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -2455,7 +2455,7 @@
         <v>43646</v>
       </c>
       <c r="B116">
-        <v>13781446268.64634</v>
+        <v>13825593044.76214</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -2463,7 +2463,7 @@
         <v>43677</v>
       </c>
       <c r="B117">
-        <v>13950792449.31811</v>
+        <v>13995753895.93792</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -2471,7 +2471,7 @@
         <v>43708</v>
       </c>
       <c r="B118">
-        <v>15078197089.83912</v>
+        <v>15128535563.3588</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -2479,7 +2479,7 @@
         <v>43738</v>
       </c>
       <c r="B119">
-        <v>14712631681.78606</v>
+        <v>14761258376.43314</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2487,7 +2487,7 @@
         <v>43769</v>
       </c>
       <c r="B120">
-        <v>14714611651.58041</v>
+        <v>14763157146.75549</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2495,7 +2495,7 @@
         <v>43799</v>
       </c>
       <c r="B121">
-        <v>14710556131.63436</v>
+        <v>14759238312.32313</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2503,7 +2503,7 @@
         <v>43830</v>
       </c>
       <c r="B122">
-        <v>14474647224.66382</v>
+        <v>14522157110.37596</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2511,7 +2511,7 @@
         <v>43861</v>
       </c>
       <c r="B123">
-        <v>15313374249.38699</v>
+        <v>15364807622.30918</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -2519,7 +2519,7 @@
         <v>43890</v>
       </c>
       <c r="B124">
-        <v>15764165624.49183</v>
+        <v>15817669589.30603</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -2527,7 +2527,7 @@
         <v>43921</v>
       </c>
       <c r="B125">
-        <v>14719289063.93287</v>
+        <v>14768230621.70415</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -2535,7 +2535,7 @@
         <v>43951</v>
       </c>
       <c r="B126">
-        <v>15671589249.38058</v>
+        <v>15724430712.58657</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -2543,7 +2543,7 @@
         <v>43982</v>
       </c>
       <c r="B127">
-        <v>15766513233.93604</v>
+        <v>15819327670.82057</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2551,7 +2551,7 @@
         <v>44012</v>
       </c>
       <c r="B128">
-        <v>15996106051.19281</v>
+        <v>16050042209.76629</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -2559,7 +2559,7 @@
         <v>44043</v>
       </c>
       <c r="B129">
-        <v>17217191287.93643</v>
+        <v>17277197553.2555</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2567,7 +2567,7 @@
         <v>44074</v>
       </c>
       <c r="B130">
-        <v>16142185864.89507</v>
+        <v>16196642282.28582</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2575,7 +2575,7 @@
         <v>44104</v>
       </c>
       <c r="B131">
-        <v>16160432747.99364</v>
+        <v>16215061226.17827</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -2583,7 +2583,7 @@
         <v>44135</v>
       </c>
       <c r="B132">
-        <v>15776376268.53454</v>
+        <v>15829096781.85946</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -2591,7 +2591,7 @@
         <v>44165</v>
       </c>
       <c r="B133">
-        <v>16592831975.27426</v>
+        <v>16649796229.19842</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2599,7 +2599,7 @@
         <v>44196</v>
       </c>
       <c r="B134">
-        <v>16526792090.92367</v>
+        <v>16583432426.03711</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -2607,7 +2607,7 @@
         <v>44227</v>
       </c>
       <c r="B135">
-        <v>15879816465.96112</v>
+        <v>15933254711.80829</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -2615,7 +2615,7 @@
         <v>44255</v>
       </c>
       <c r="B136">
-        <v>15138477358.95779</v>
+        <v>15188499974.49528</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2623,7 +2623,7 @@
         <v>44286</v>
       </c>
       <c r="B137">
-        <v>14529082665.88137</v>
+        <v>14576418210.54709</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2631,7 +2631,7 @@
         <v>44316</v>
       </c>
       <c r="B138">
-        <v>14881417766.51148</v>
+        <v>14930378222.98885</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2639,7 +2639,7 @@
         <v>44347</v>
       </c>
       <c r="B139">
-        <v>14921733749.02908</v>
+        <v>14970810418.37663</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2647,7 +2647,7 @@
         <v>44377</v>
       </c>
       <c r="B140">
-        <v>15562232593.29958</v>
+        <v>15614564429.2749</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2655,7 +2655,7 @@
         <v>44408</v>
       </c>
       <c r="B141">
-        <v>15948867648.82611</v>
+        <v>16002984187.24857</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2663,7 +2663,7 @@
         <v>44439</v>
       </c>
       <c r="B142">
-        <v>15803124885.51801</v>
+        <v>15856596259.62006</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2671,7 +2671,7 @@
         <v>44469</v>
       </c>
       <c r="B143">
-        <v>15446071532.90326</v>
+        <v>15497894914.94207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>